<commit_message>
Preparing to add new supplemental figures with annotations on backbone.
</commit_message>
<xml_diff>
--- a/figureS7_sweep_dynamics/site_transitions.xlsx
+++ b/figureS7_sweep_dynamics/site_transitions.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA6A45D-C57D-4726-8D7A-EFB9C4F30321}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="transitional_list" sheetId="1" r:id="rId1"/>
@@ -28,21 +29,12 @@
     <t>98A</t>
   </si>
   <si>
-    <t>I3L,T5A,I12T,V16I,Y26C,N29H,N33T,I48T,E50K,K50R,I63K,K79R,N127D,D133N,V135F,I151V,K173R,K185E,E185N,M227V,R235I,I249V,L255I,V299A,R317I,I317K</t>
-  </si>
-  <si>
     <t>02A</t>
   </si>
   <si>
     <t>02B</t>
   </si>
   <si>
-    <t>L8F,N27D,V36A,M37I,K61R,D72S,K79N,D113G,I135V,S147N,I162M,I180V,D185N,F191L,I243V,V249I,I249V,R250H,K253T,Y270F,D295N,H296Y,V298I,N315S,S315N,L318F,F318V,H322Y</t>
-  </si>
-  <si>
-    <t>I12V,V12I,D27N,N29D,Q35H,L38F,K48T,I59V,L67P,A68T,I243V,I249V,I298T</t>
-  </si>
-  <si>
     <t>S43N,N86I,N141S,D147G,V165I,T238A,I254V,I265T,V307I</t>
   </si>
   <si>
@@ -269,12 +261,21 @@
   </si>
   <si>
     <t>NA Clade</t>
+  </si>
+  <si>
+    <t>V13I,I17L,T19A,V30I,Y40C,N43H,N47T,I62T,E64K,K64N,I77K,K93R,D147N,V149F,I165V,K187R,E199N,K199E, M241V,R249I,I263V,L269I,V313A</t>
+  </si>
+  <si>
+    <t>L22F,N41D,V50A,M51I,K75R,D86S,K93N,D127G,I149V,S161N,I176M,I194V,D199N,F205L,I257V,V263I,I263V,R264H,K267T,S284F,D309N,H310Y,V312I</t>
+  </si>
+  <si>
+    <t>I26V,V26I,D41N,N43D,Q49H,L52F,K62T,I73V,L81P,A82T,I257V,I263V,I312T</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -373,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -400,6 +401,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -680,11 +684,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B5"/>
+      <selection activeCell="B5" sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,42 +699,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>2</v>
+        <v>76</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -740,7 +744,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
@@ -760,130 +764,130 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C11" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -891,21 +895,21 @@
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -915,7 +919,7 @@
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -923,92 +927,92 @@
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="5"/>
       <c r="E25" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1017,48 +1021,48 @@
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B34" s="2"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1066,14 +1070,14 @@
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1083,29 +1087,29 @@
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D44" s="2"/>
     </row>
@@ -1113,13 +1117,13 @@
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D45" s="2"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1128,14 +1132,14 @@
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -1145,7 +1149,7 @@
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D49" s="2"/>
     </row>
@@ -1153,7 +1157,7 @@
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D50" s="2"/>
     </row>
@@ -1161,7 +1165,7 @@
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D51" s="2"/>
     </row>
@@ -1169,41 +1173,41 @@
       <c r="A52" s="3"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D53" s="2"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C55" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C58" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>